<commit_message>
checks ans downloads 5.1
</commit_message>
<xml_diff>
--- a/ontwikkeling/voorstel 5.1/5.1 checks.xlsx
+++ b/ontwikkeling/voorstel 5.1/5.1 checks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\100289\OneDrive\GitHub\NLCS\ontwikkeling\voorstel 5.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FA5DD6-F342-41B1-803D-5D7194A1DA34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29144C6-38B6-4D37-B43E-59FF88C96F8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9600" yWindow="0" windowWidth="9600" windowHeight="10200" xr2:uid="{E7E2FD8D-6DE2-496D-85F1-D19C23E418FB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E7E2FD8D-6DE2-496D-85F1-D19C23E418FB}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="96">
   <si>
     <t>Kleuren</t>
   </si>
@@ -304,6 +304,30 @@
   </si>
   <si>
     <t>als tijd, aanpassen kleuren nav michel</t>
+  </si>
+  <si>
+    <t>OBJECTENTABEL VERKORT</t>
+  </si>
+  <si>
+    <t>OBJECTENTABEL LANG</t>
+  </si>
+  <si>
+    <t>FF 1 HANDMATIG INVULLEN</t>
+  </si>
+  <si>
+    <t>ONBEGRIJPELIJKE GEBREKEN IN PUBLICATIE V</t>
+  </si>
+  <si>
+    <t>FF 2 HANDMATIG INVULLEN</t>
+  </si>
+  <si>
+    <t>CSV UPDATEN</t>
+  </si>
+  <si>
+    <t>SAM-AS-SPOOR</t>
+  </si>
+  <si>
+    <t>SPOORSE OBJECTEN</t>
   </si>
 </sst>
 </file>
@@ -706,7 +730,7 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -716,6 +740,7 @@
     <col min="4" max="4" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.7265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
@@ -737,6 +762,12 @@
       <c r="F1" t="s">
         <v>10</v>
       </c>
+      <c r="G1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="H1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -747,6 +778,10 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="K2" t="s">
         <v>52</v>
       </c>
@@ -760,6 +795,10 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
+      <c r="G3" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="1"/>
       <c r="K3" t="s">
         <v>53</v>
       </c>
@@ -773,6 +812,8 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
       <c r="K4" t="s">
         <v>54</v>
       </c>
@@ -786,6 +827,8 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
       <c r="K5" t="s">
         <v>55</v>
       </c>
@@ -801,7 +844,8 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
       <c r="K6" t="s">
         <v>56</v>
       </c>
@@ -815,6 +859,8 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
       <c r="K7" t="s">
         <v>57</v>
       </c>
@@ -823,15 +869,13 @@
       <c r="A8" t="s">
         <v>44</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
       <c r="K8" t="s">
         <v>58</v>
       </c>
@@ -845,6 +889,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
+      <c r="H9" s="1"/>
       <c r="K9" t="s">
         <v>59</v>
       </c>
@@ -853,15 +898,12 @@
       <c r="A10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
+      <c r="H10" s="1"/>
       <c r="K10" t="s">
         <v>60</v>
       </c>
@@ -870,15 +912,12 @@
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
+      <c r="H11" s="2"/>
       <c r="K11" t="s">
         <v>61</v>
       </c>
@@ -887,15 +926,12 @@
       <c r="A12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
+      <c r="H12" s="2"/>
       <c r="K12" t="s">
         <v>62</v>
       </c>
@@ -909,6 +945,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
+      <c r="H13" s="1"/>
       <c r="K13" t="s">
         <v>63</v>
       </c>
@@ -922,6 +959,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
+      <c r="H14" s="1"/>
       <c r="K14" t="s">
         <v>64</v>
       </c>
@@ -930,19 +968,12 @@
       <c r="A15" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="F15" s="1"/>
+      <c r="H15" s="2"/>
       <c r="K15" t="s">
         <v>65</v>
       </c>
@@ -958,7 +989,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="3"/>
+      <c r="H16" s="2"/>
       <c r="K16" t="s">
         <v>66</v>
       </c>
@@ -972,7 +1003,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="3"/>
+      <c r="H17" s="1"/>
       <c r="K17" t="s">
         <v>67</v>
       </c>
@@ -981,18 +1012,12 @@
       <c r="A18" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="3"/>
+      <c r="F18" s="1"/>
+      <c r="H18" s="2"/>
       <c r="K18" t="s">
         <v>68</v>
       </c>
@@ -1006,6 +1031,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
+      <c r="H19" s="1"/>
       <c r="K19" t="s">
         <v>69</v>
       </c>
@@ -1023,6 +1049,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
+      <c r="H20" s="2"/>
       <c r="K20" t="s">
         <v>70</v>
       </c>
@@ -1031,12 +1058,12 @@
       <c r="A21" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="H21" s="2"/>
       <c r="K21" t="s">
         <v>71</v>
       </c>
@@ -1045,15 +1072,12 @@
       <c r="A22" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
+      <c r="H22" s="1"/>
       <c r="K22" t="s">
         <v>72</v>
       </c>
@@ -1067,6 +1091,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
+      <c r="H23" s="1"/>
       <c r="K23" t="s">
         <v>73</v>
       </c>
@@ -1084,6 +1109,7 @@
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
+      <c r="H24" s="2"/>
       <c r="K24" t="s">
         <v>74</v>
       </c>
@@ -1097,6 +1123,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
+      <c r="H25" s="1"/>
       <c r="K25" t="s">
         <v>75</v>
       </c>
@@ -1114,6 +1141,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
+      <c r="H26" s="1"/>
       <c r="K26" t="s">
         <v>76</v>
       </c>
@@ -1129,6 +1157,7 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
+      <c r="H27" s="2"/>
       <c r="K27" t="s">
         <v>77</v>
       </c>
@@ -1142,6 +1171,7 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
+      <c r="H28" s="1"/>
       <c r="K28" t="s">
         <v>78</v>
       </c>
@@ -1150,16 +1180,15 @@
       <c r="A29" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="3"/>
+      <c r="G29" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H29" s="1"/>
       <c r="K29" t="s">
         <v>79</v>
       </c>
@@ -1175,7 +1204,7 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="3"/>
+      <c r="H30" s="2"/>
       <c r="K30" t="s">
         <v>80</v>
       </c>
@@ -1189,6 +1218,7 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
+      <c r="H31" s="1"/>
       <c r="K31" t="s">
         <v>81</v>
       </c>
@@ -1202,7 +1232,9 @@
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
+      <c r="H32" s="2" t="s">
+        <v>91</v>
+      </c>
       <c r="K32" t="s">
         <v>82</v>
       </c>
@@ -1220,7 +1252,7 @@
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+      <c r="H33" s="1"/>
       <c r="K33" t="s">
         <v>83</v>
       </c>
@@ -1229,8 +1261,17 @@
       <c r="A34" t="s">
         <v>40</v>
       </c>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>93</v>
+      </c>
       <c r="K34" t="s">
         <v>84</v>
       </c>
@@ -1239,8 +1280,12 @@
       <c r="A35" t="s">
         <v>41</v>
       </c>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="H35" s="1"/>
       <c r="K35" t="s">
         <v>85</v>
       </c>
@@ -1249,8 +1294,12 @@
       <c r="A36" t="s">
         <v>42</v>
       </c>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="H36" s="2"/>
       <c r="K36" t="s">
         <v>86</v>
       </c>

</xml_diff>